<commit_message>
INdex and match functions added
</commit_message>
<xml_diff>
--- a/Lookup and Reference functions.xlsx
+++ b/Lookup and Reference functions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Learning Data analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85E7563-7572-4291-ADBB-717E9C474213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00F7352-240A-4AD7-886F-8CCCFA0B5C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E91A5715-09BE-49EC-A6FC-BA5DB67F179C}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{E91A5715-09BE-49EC-A6FC-BA5DB67F179C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -67,6 +68,18 @@
   </si>
   <si>
     <t>Math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salary </t>
+  </si>
+  <si>
+    <t>Workexp</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>match</t>
   </si>
 </sst>
 </file>
@@ -420,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A609F18-3B48-44D1-9502-D08F10274F4D}">
   <dimension ref="C3:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -577,4 +590,92 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E25047A-3381-44AF-9B2C-9ABABE56808B}">
+  <dimension ref="C3:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>30000</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>25000</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>35000</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>32000</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f>INDEX(C3:E7,4,3)</f>
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>MATCH(C4,C3:C7,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>